<commit_message>
updated the Question spreadsheet
</commit_message>
<xml_diff>
--- a/SamsungAPI2/Assets/Spreadsheets/SamsungQuestions.xlsx
+++ b/SamsungAPI2/Assets/Spreadsheets/SamsungQuestions.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timbo\RiderProjects\SamsungAPI2\SamsungAPI2\Assets\Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\timbo\dev\Source\Repos\samsung-questions-intuiface\SamsungAPI2\bin\Debug\netstandard2.0\Assets\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785B8B25-CA95-4426-B270-A1986E416168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A8E8FC-228F-46EC-9576-21FAF99F1368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="1560" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3825" yWindow="2070" windowWidth="21600" windowHeight="12735" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Laptops" sheetId="1" r:id="rId1"/>
-    <sheet name="Modiles" sheetId="2" r:id="rId2"/>
-    <sheet name="Tablets" sheetId="3" r:id="rId3"/>
-    <sheet name="Hearable" sheetId="4" r:id="rId4"/>
-    <sheet name="Wearable" sheetId="5" r:id="rId5"/>
+    <sheet name="Tablets" sheetId="3" r:id="rId2"/>
+    <sheet name="Mobiles" sheetId="2" r:id="rId3"/>
+    <sheet name="Wearables" sheetId="5" r:id="rId4"/>
+    <sheet name="Hearables" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
   <si>
     <t>Question</t>
   </si>
@@ -125,13 +125,211 @@
   </si>
   <si>
     <t>Checkbox</t>
+  </si>
+  <si>
+    <t>Question Text</t>
+  </si>
+  <si>
+    <t>Answer Text</t>
+  </si>
+  <si>
+    <t>Best in class display</t>
+  </si>
+  <si>
+    <t>Samsung Kids Mode</t>
+  </si>
+  <si>
+    <t>Attach a keyboard</t>
+  </si>
+  <si>
+    <t>Smaller Display (8"- 10")</t>
+  </si>
+  <si>
+    <t>Larger Display (11"+)</t>
+  </si>
+  <si>
+    <t>Kids</t>
+  </si>
+  <si>
+    <t>I want the tablet to be…</t>
+  </si>
+  <si>
+    <t>I want to use the tablet for…</t>
+  </si>
+  <si>
+    <t>Skittles 1</t>
+  </si>
+  <si>
+    <t>Skittles 2 </t>
+  </si>
+  <si>
+    <t>Skittles 3</t>
+  </si>
+  <si>
+    <t>Tab A7 Grey</t>
+  </si>
+  <si>
+    <t>Tab A7 Lite Black</t>
+  </si>
+  <si>
+    <t>Tab S6 Lite Blue (With Keyboard &amp; Spen)</t>
+  </si>
+  <si>
+    <t>Tab S7 Black (with Keyboard &amp; Spen)</t>
+  </si>
+  <si>
+    <t>Tab S7+ Navy (with Keyboard &amp; Spen)</t>
+  </si>
+  <si>
+    <t>Tab S7FE Black</t>
+  </si>
+  <si>
+    <t>Tab S7FE Green (with Spen)</t>
+  </si>
+  <si>
+    <t>Tab S7FE Silver (with Spen)</t>
+  </si>
+  <si>
+    <t>Answer Id</t>
+  </si>
+  <si>
+    <t>I want the mobile to be…</t>
+  </si>
+  <si>
+    <t>I want to use the mobile for…</t>
+  </si>
+  <si>
+    <t>I want the wearable to be…</t>
+  </si>
+  <si>
+    <t>I want to use the wearable for…</t>
+  </si>
+  <si>
+    <t>Track step count</t>
+  </si>
+  <si>
+    <t>Track workouts</t>
+  </si>
+  <si>
+    <t>Track Heart rate</t>
+  </si>
+  <si>
+    <t>Record Body Composition</t>
+  </si>
+  <si>
+    <t>Monitor Blood pressure/ECG</t>
+  </si>
+  <si>
+    <t>Receive calls and notifications</t>
+  </si>
+  <si>
+    <t>Store &amp; listen to music</t>
+  </si>
+  <si>
+    <t>Water/Sweat Resistance</t>
+  </si>
+  <si>
+    <t>A minimalist design</t>
+  </si>
+  <si>
+    <t>A classic watch design</t>
+  </si>
+  <si>
+    <t>Larger in size</t>
+  </si>
+  <si>
+    <t>Smaller in size</t>
+  </si>
+  <si>
+    <t>4G Connected</t>
+  </si>
+  <si>
+    <t>Running/Working out</t>
+  </si>
+  <si>
+    <t>Receiving notifcations</t>
+  </si>
+  <si>
+    <t>Contactless payments</t>
+  </si>
+  <si>
+    <t>Galaxy Watch 4 40mm Gold</t>
+  </si>
+  <si>
+    <t>Galaxy Watch 4 44mm Black BT</t>
+  </si>
+  <si>
+    <t>Galaxy Watch 4 44mm Green</t>
+  </si>
+  <si>
+    <t>Galaxy Watch 4 Classic 42mm Black</t>
+  </si>
+  <si>
+    <t>Galaxy Watch 4 Classic 46mm  Silver</t>
+  </si>
+  <si>
+    <t>I want the hearable to be…</t>
+  </si>
+  <si>
+    <t>I want to use the hearable for…</t>
+  </si>
+  <si>
+    <t>Active Noise Cancelling</t>
+  </si>
+  <si>
+    <t>Ambient Sound</t>
+  </si>
+  <si>
+    <t>Best in class sound quality</t>
+  </si>
+  <si>
+    <t>Water/Sweat Resistant</t>
+  </si>
+  <si>
+    <t>360 Audio</t>
+  </si>
+  <si>
+    <t>Wireless Charging</t>
+  </si>
+  <si>
+    <t>Use across multiple devices</t>
+  </si>
+  <si>
+    <t>Canal type (inside ear canal)</t>
+  </si>
+  <si>
+    <t>Open type (sit on ear)</t>
+  </si>
+  <si>
+    <t>Music &amp; Podcasts</t>
+  </si>
+  <si>
+    <t>Phone/video calls</t>
+  </si>
+  <si>
+    <t>Gaming</t>
+  </si>
+  <si>
+    <t>Buds 2 Black</t>
+  </si>
+  <si>
+    <t>Buds 2 White</t>
+  </si>
+  <si>
+    <t>Buds Live Black</t>
+  </si>
+  <si>
+    <t>Buds Pro Black</t>
+  </si>
+  <si>
+    <t>Buds Pro Violet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,8 +351,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +382,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -235,6 +453,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,49 +1261,2076 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4">
+        <v>2</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>2</v>
+      </c>
+      <c r="N2" s="4">
+        <v>2</v>
+      </c>
+      <c r="O2" s="4">
+        <v>2</v>
+      </c>
+      <c r="P2" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>2</v>
+      </c>
+      <c r="R2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="13">
+        <v>2</v>
+      </c>
+      <c r="G3" s="13">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4">
+        <v>2</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>1</v>
+      </c>
+      <c r="O3" s="4">
+        <v>2</v>
+      </c>
+      <c r="P3" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>1</v>
+      </c>
+      <c r="R3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="13">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2</v>
+      </c>
+      <c r="J4" s="4">
+        <v>2</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="4">
+        <v>2</v>
+      </c>
+      <c r="O4" s="4">
+        <v>2</v>
+      </c>
+      <c r="P4" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>2</v>
+      </c>
+      <c r="R4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="13">
+        <v>4</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1</v>
+      </c>
+      <c r="P5" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>1</v>
+      </c>
+      <c r="R5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="13">
+        <v>5</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>2</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2</v>
+      </c>
+      <c r="N6" s="4">
+        <v>2</v>
+      </c>
+      <c r="O6" s="4">
+        <v>2</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>2</v>
+      </c>
+      <c r="R6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>2</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="13">
+        <v>6</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+      <c r="M7" s="4">
+        <v>2</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>0</v>
+      </c>
+      <c r="R7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="13">
+        <v>7</v>
+      </c>
+      <c r="G8" s="13">
+        <v>2</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2</v>
+      </c>
+      <c r="J8" s="4">
+        <v>2</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>2</v>
+      </c>
+      <c r="O8" s="4">
+        <v>2</v>
+      </c>
+      <c r="P8" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>2</v>
+      </c>
+      <c r="R8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="11">
+        <v>3</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="13">
+        <v>8</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2</v>
+      </c>
+      <c r="I9" s="4">
+        <v>2</v>
+      </c>
+      <c r="J9" s="4">
+        <v>2</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="4">
+        <v>2</v>
+      </c>
+      <c r="O9" s="4">
+        <v>2</v>
+      </c>
+      <c r="P9" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>2</v>
+      </c>
+      <c r="R9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11">
+        <v>3</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="13">
+        <v>9</v>
+      </c>
+      <c r="G10" s="13">
+        <v>2</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2</v>
+      </c>
+      <c r="I10" s="4">
+        <v>2</v>
+      </c>
+      <c r="J10" s="4">
+        <v>2</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>2</v>
+      </c>
+      <c r="N10" s="4">
+        <v>2</v>
+      </c>
+      <c r="O10" s="4">
+        <v>2</v>
+      </c>
+      <c r="P10" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>2</v>
+      </c>
+      <c r="R10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>3</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="13">
+        <v>10</v>
+      </c>
+      <c r="G11" s="13">
+        <v>3</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4">
+        <v>2</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2</v>
+      </c>
+      <c r="M11" s="4">
+        <v>2</v>
+      </c>
+      <c r="N11" s="4">
+        <v>1</v>
+      </c>
+      <c r="O11" s="4">
+        <v>1</v>
+      </c>
+      <c r="P11" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>1</v>
+      </c>
+      <c r="R11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11">
+        <v>3</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="13">
+        <v>11</v>
+      </c>
+      <c r="G12" s="13">
+        <v>4</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>2</v>
+      </c>
+      <c r="L12" s="4">
+        <v>2</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>0</v>
+      </c>
+      <c r="R12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="B18:B25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4">
+        <v>2</v>
+      </c>
+      <c r="L2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="13">
+        <v>2</v>
+      </c>
+      <c r="G3" s="13">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
+        <v>2</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>1</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="13">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="13">
+        <v>4</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>1</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="13">
+        <v>5</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2</v>
+      </c>
+      <c r="L6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>1</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="13">
+        <v>6</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>2</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2</v>
+      </c>
+      <c r="J7" s="4">
+        <v>2</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="13">
+        <v>7</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2</v>
+      </c>
+      <c r="J8" s="4">
+        <v>2</v>
+      </c>
+      <c r="K8" s="4">
+        <v>2</v>
+      </c>
+      <c r="L8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>2</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="13">
+        <v>2</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="13">
+        <v>8</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2</v>
+      </c>
+      <c r="I9" s="4">
+        <v>2</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>2</v>
+      </c>
+      <c r="L9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>2</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="13">
+        <v>2</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="13">
+        <v>9</v>
+      </c>
+      <c r="G10" s="13">
+        <v>2</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>2</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>3</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="13">
+        <v>3</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="13">
+        <v>10</v>
+      </c>
+      <c r="G11" s="13">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>2</v>
+      </c>
+      <c r="J11" s="4">
+        <v>2</v>
+      </c>
+      <c r="K11" s="4">
+        <v>2</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>3</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="13">
+        <v>3</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="13">
+        <v>11</v>
+      </c>
+      <c r="G12" s="13">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1</v>
+      </c>
+      <c r="K12" s="4">
+        <v>2</v>
+      </c>
+      <c r="L12" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="13">
+        <v>12</v>
+      </c>
+      <c r="G13" s="13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2</v>
+      </c>
+      <c r="L13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>3</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="13">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="13">
+        <v>13</v>
+      </c>
+      <c r="G14" s="13">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>2</v>
+      </c>
+      <c r="L14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15">
+        <v>2</v>
+      </c>
+      <c r="I2" s="15">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4">
+        <v>2</v>
+      </c>
+      <c r="K2" s="4">
+        <v>2</v>
+      </c>
+      <c r="L2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="13">
+        <v>2</v>
+      </c>
+      <c r="G3" s="13">
+        <v>1</v>
+      </c>
+      <c r="H3" s="15">
+        <v>2</v>
+      </c>
+      <c r="I3" s="15">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4">
+        <v>2</v>
+      </c>
+      <c r="K3" s="4">
+        <v>2</v>
+      </c>
+      <c r="L3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>1</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="13">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="H4" s="15">
+        <v>2</v>
+      </c>
+      <c r="I4" s="15">
+        <v>2</v>
+      </c>
+      <c r="J4" s="4">
+        <v>2</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="13">
+        <v>4</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="H5" s="15">
+        <v>2</v>
+      </c>
+      <c r="I5" s="15">
+        <v>2</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>1</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="13">
+        <v>5</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="15">
+        <v>2</v>
+      </c>
+      <c r="I6" s="15">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>2</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2</v>
+      </c>
+      <c r="L6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>1</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="13">
+        <v>6</v>
+      </c>
+      <c r="G7" s="13">
+        <v>11</v>
+      </c>
+      <c r="H7" s="15">
+        <v>2</v>
+      </c>
+      <c r="I7" s="15">
+        <v>2</v>
+      </c>
+      <c r="J7" s="4">
+        <v>2</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="13">
+        <v>7</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2</v>
+      </c>
+      <c r="J8" s="4">
+        <v>2</v>
+      </c>
+      <c r="K8" s="4">
+        <v>2</v>
+      </c>
+      <c r="L8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>1</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="13">
+        <v>8</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2</v>
+      </c>
+      <c r="I9" s="4">
+        <v>2</v>
+      </c>
+      <c r="J9" s="4">
+        <v>2</v>
+      </c>
+      <c r="K9" s="4">
+        <v>2</v>
+      </c>
+      <c r="L9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>2</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="13">
+        <v>2</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="13">
+        <v>9</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2</v>
+      </c>
+      <c r="I10" s="4">
+        <v>2</v>
+      </c>
+      <c r="J10" s="4">
+        <v>2</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>2</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="13">
+        <v>2</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="13">
+        <v>10</v>
+      </c>
+      <c r="G11" s="13">
+        <v>2</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>2</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>2</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="13">
+        <v>2</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="13">
+        <v>11</v>
+      </c>
+      <c r="G12" s="13">
+        <v>3</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>2</v>
+      </c>
+      <c r="J12" s="4">
+        <v>2</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="13">
+        <v>12</v>
+      </c>
+      <c r="G13" s="13">
+        <v>4</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>2</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="13">
+        <v>2</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="13">
+        <v>13</v>
+      </c>
+      <c r="G14" s="13">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>3</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="13">
+        <v>3</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="13">
+        <v>14</v>
+      </c>
+      <c r="G15" s="13">
+        <v>1</v>
+      </c>
+      <c r="H15" s="15">
+        <v>2</v>
+      </c>
+      <c r="I15" s="15">
+        <v>2</v>
+      </c>
+      <c r="J15" s="4">
+        <v>2</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>3</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="13">
+        <v>3</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="13">
+        <v>15</v>
+      </c>
+      <c r="G16" s="13">
+        <v>2</v>
+      </c>
+      <c r="H16" s="15">
+        <v>2</v>
+      </c>
+      <c r="I16" s="15">
+        <v>2</v>
+      </c>
+      <c r="J16" s="4">
+        <v>2</v>
+      </c>
+      <c r="K16" s="4">
+        <v>2</v>
+      </c>
+      <c r="L16" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>3</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="13">
+        <v>3</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="13">
+        <v>16</v>
+      </c>
+      <c r="G17" s="13">
+        <v>3</v>
+      </c>
+      <c r="H17" s="15">
+        <v>2</v>
+      </c>
+      <c r="I17" s="15">
+        <v>2</v>
+      </c>
+      <c r="J17" s="4">
+        <v>2</v>
+      </c>
+      <c r="K17" s="4">
+        <v>2</v>
+      </c>
+      <c r="L17" s="4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B15:B17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>